<commit_message>
Upload from Ant 1
</commit_message>
<xml_diff>
--- a/Warehouse/00Inbox/模型搜索.xlsx
+++ b/Warehouse/00Inbox/模型搜索.xlsx
@@ -108,9 +108,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
@@ -122,8 +122,23 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -138,74 +153,77 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF3F3F76"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -219,6 +237,20 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
@@ -227,40 +259,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -275,187 +275,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -466,6 +466,15 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -480,6 +489,60 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -503,69 +566,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -574,10 +574,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -586,133 +586,133 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="14" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="25" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -824,15 +824,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>657225</xdr:colOff>
+      <xdr:colOff>647700</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>26</xdr:col>
-      <xdr:colOff>686435</xdr:colOff>
+      <xdr:colOff>676275</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>153035</xdr:rowOff>
+      <xdr:rowOff>172085</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -849,8 +849,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="13001625" y="133350"/>
-          <a:ext cx="5515610" cy="3105785"/>
+          <a:off x="12992100" y="152400"/>
+          <a:ext cx="5514975" cy="3105785"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -864,13 +864,13 @@
       <xdr:col>18</xdr:col>
       <xdr:colOff>390525</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>26</xdr:col>
       <xdr:colOff>175895</xdr:colOff>
       <xdr:row>38</xdr:row>
-      <xdr:rowOff>66040</xdr:rowOff>
+      <xdr:rowOff>75565</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -887,7 +887,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="12734925" y="3286125"/>
+          <a:off x="12734925" y="3295650"/>
           <a:ext cx="5271770" cy="3295015"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1161,7 +1161,7 @@
   <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M33" sqref="M33"/>
+      <selection activeCell="M15" sqref="M15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="6"/>

</xml_diff>